<commit_message>
Nuevos datos entre julio 2021 hasta diciembre 2021
</commit_message>
<xml_diff>
--- a/data/ToneladasBiosanitariosAMB.xlsx
+++ b/data/ToneladasBiosanitariosAMB.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tesis\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675AE2E8-5873-4CDE-B04A-02E6BF67F184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D5C443D-7FEB-4C38-9CAE-3F4D19A614DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,11 +44,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.00000E+00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,9 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,14 +402,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619AC86B-519F-428A-87AA-46C5CD2A3EAC}">
-  <dimension ref="A1:B396"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="K16" sqref="K15:K16"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="D386" sqref="D386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3472,7 +3486,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>44366</v>
       </c>
@@ -3480,7 +3494,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>44367</v>
       </c>
@@ -3488,7 +3502,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>44368</v>
       </c>
@@ -3496,7 +3510,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>44369</v>
       </c>
@@ -3504,7 +3518,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>44370</v>
       </c>
@@ -3512,7 +3526,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>44371</v>
       </c>
@@ -3520,7 +3534,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>44372</v>
       </c>
@@ -3528,7 +3542,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>44373</v>
       </c>
@@ -3536,7 +3550,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>44374</v>
       </c>
@@ -3544,7 +3558,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>44375</v>
       </c>
@@ -3552,7 +3566,7 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>44376</v>
       </c>
@@ -3560,12 +3574,1486 @@
         <v>4.6399036666666662</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>44377</v>
       </c>
       <c r="B396">
         <v>4.6399036666666662</v>
+      </c>
+      <c r="F396" s="3"/>
+      <c r="G396" s="3"/>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A397" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B397">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A398" s="1">
+        <v>44379</v>
+      </c>
+      <c r="B398">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A399" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B399">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A400" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B400">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" s="1">
+        <v>44382</v>
+      </c>
+      <c r="B401">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B402">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="1">
+        <v>44384</v>
+      </c>
+      <c r="B403">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="1">
+        <v>44385</v>
+      </c>
+      <c r="B404">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="1">
+        <v>44386</v>
+      </c>
+      <c r="B405">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" s="1">
+        <v>44387</v>
+      </c>
+      <c r="B406">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" s="1">
+        <v>44388</v>
+      </c>
+      <c r="B407">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" s="1">
+        <v>44389</v>
+      </c>
+      <c r="B408">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="1">
+        <v>44390</v>
+      </c>
+      <c r="B409">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" s="1">
+        <v>44391</v>
+      </c>
+      <c r="B410">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B411">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" s="1">
+        <v>44393</v>
+      </c>
+      <c r="B412">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" s="1">
+        <v>44394</v>
+      </c>
+      <c r="B413">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" s="1">
+        <v>44395</v>
+      </c>
+      <c r="B414">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B415">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" s="1">
+        <v>44397</v>
+      </c>
+      <c r="B416">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" s="1">
+        <v>44398</v>
+      </c>
+      <c r="B417">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" s="1">
+        <v>44399</v>
+      </c>
+      <c r="B418">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" s="1">
+        <v>44400</v>
+      </c>
+      <c r="B419">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" s="1">
+        <v>44401</v>
+      </c>
+      <c r="B420">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" s="1">
+        <v>44402</v>
+      </c>
+      <c r="B421">
+        <v>3.0519926666666666</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" s="1">
+        <v>44403</v>
+      </c>
+      <c r="B422">
+        <v>3.0519926666666701</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" s="1">
+        <v>44404</v>
+      </c>
+      <c r="B423">
+        <v>3.0519926666666701</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" s="1">
+        <v>44405</v>
+      </c>
+      <c r="B424">
+        <v>3.0519926666666701</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" s="1">
+        <v>44406</v>
+      </c>
+      <c r="B425">
+        <v>3.0519926666666701</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" s="1">
+        <v>44407</v>
+      </c>
+      <c r="B426">
+        <v>3.0519926666666701</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" s="1">
+        <v>44408</v>
+      </c>
+      <c r="B427">
+        <v>3.0519926666666701</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B428">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B429">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B430">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" s="1">
+        <v>44412</v>
+      </c>
+      <c r="B431">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="1">
+        <v>44413</v>
+      </c>
+      <c r="B432">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="1">
+        <v>44414</v>
+      </c>
+      <c r="B433">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="1">
+        <v>44415</v>
+      </c>
+      <c r="B434">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="1">
+        <v>44416</v>
+      </c>
+      <c r="B435">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="1">
+        <v>44417</v>
+      </c>
+      <c r="B436">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="1">
+        <v>44418</v>
+      </c>
+      <c r="B437">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="1">
+        <v>44419</v>
+      </c>
+      <c r="B438">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="1">
+        <v>44420</v>
+      </c>
+      <c r="B439">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="1">
+        <v>44421</v>
+      </c>
+      <c r="B440">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="1">
+        <v>44422</v>
+      </c>
+      <c r="B441">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="1">
+        <v>44423</v>
+      </c>
+      <c r="B442">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B443">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="1">
+        <v>44425</v>
+      </c>
+      <c r="B444">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" s="1">
+        <v>44426</v>
+      </c>
+      <c r="B445">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="1">
+        <v>44427</v>
+      </c>
+      <c r="B446">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" s="1">
+        <v>44428</v>
+      </c>
+      <c r="B447">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" s="1">
+        <v>44429</v>
+      </c>
+      <c r="B448">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" s="1">
+        <v>44430</v>
+      </c>
+      <c r="B449">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" s="1">
+        <v>44431</v>
+      </c>
+      <c r="B450">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" s="1">
+        <v>44432</v>
+      </c>
+      <c r="B451">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" s="1">
+        <v>44433</v>
+      </c>
+      <c r="B452">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" s="1">
+        <v>44434</v>
+      </c>
+      <c r="B453">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" s="1">
+        <v>44435</v>
+      </c>
+      <c r="B454">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" s="1">
+        <v>44436</v>
+      </c>
+      <c r="B455">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" s="1">
+        <v>44437</v>
+      </c>
+      <c r="B456">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" s="1">
+        <v>44438</v>
+      </c>
+      <c r="B457">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" s="1">
+        <v>44439</v>
+      </c>
+      <c r="B458">
+        <v>1.2497473333333335</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B459">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" s="1">
+        <v>44441</v>
+      </c>
+      <c r="B460">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" s="1">
+        <v>44442</v>
+      </c>
+      <c r="B461">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B462">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" s="1">
+        <v>44444</v>
+      </c>
+      <c r="B463">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" s="1">
+        <v>44445</v>
+      </c>
+      <c r="B464">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" s="1">
+        <v>44446</v>
+      </c>
+      <c r="B465">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" s="1">
+        <v>44447</v>
+      </c>
+      <c r="B466">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" s="1">
+        <v>44448</v>
+      </c>
+      <c r="B467">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" s="1">
+        <v>44449</v>
+      </c>
+      <c r="B468">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B469">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" s="1">
+        <v>44451</v>
+      </c>
+      <c r="B470">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" s="1">
+        <v>44452</v>
+      </c>
+      <c r="B471">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" s="1">
+        <v>44453</v>
+      </c>
+      <c r="B472">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" s="1">
+        <v>44454</v>
+      </c>
+      <c r="B473">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B474">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" s="1">
+        <v>44456</v>
+      </c>
+      <c r="B475">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" s="1">
+        <v>44457</v>
+      </c>
+      <c r="B476">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" s="1">
+        <v>44458</v>
+      </c>
+      <c r="B477">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B478">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" s="1">
+        <v>44460</v>
+      </c>
+      <c r="B479">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" s="1">
+        <v>44461</v>
+      </c>
+      <c r="B480">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" s="1">
+        <v>44462</v>
+      </c>
+      <c r="B481">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" s="1">
+        <v>44463</v>
+      </c>
+      <c r="B482">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" s="1">
+        <v>44464</v>
+      </c>
+      <c r="B483">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" s="1">
+        <v>44465</v>
+      </c>
+      <c r="B484">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" s="1">
+        <v>44466</v>
+      </c>
+      <c r="B485">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" s="1">
+        <v>44467</v>
+      </c>
+      <c r="B486">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" s="1">
+        <v>44468</v>
+      </c>
+      <c r="B487">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B488">
+        <v>1.6654793333333335</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B489" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A490" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B490" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" s="1">
+        <v>44472</v>
+      </c>
+      <c r="B491" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" s="1">
+        <v>44473</v>
+      </c>
+      <c r="B492" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" s="1">
+        <v>44474</v>
+      </c>
+      <c r="B493" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494" s="1">
+        <v>44475</v>
+      </c>
+      <c r="B494" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" s="1">
+        <v>44476</v>
+      </c>
+      <c r="B495" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" s="1">
+        <v>44477</v>
+      </c>
+      <c r="B496" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" s="1">
+        <v>44478</v>
+      </c>
+      <c r="B497" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" s="1">
+        <v>44479</v>
+      </c>
+      <c r="B498" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" s="1">
+        <v>44480</v>
+      </c>
+      <c r="B499" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" s="1">
+        <v>44481</v>
+      </c>
+      <c r="B500" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A501" s="1">
+        <v>44482</v>
+      </c>
+      <c r="B501" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A502" s="1">
+        <v>44483</v>
+      </c>
+      <c r="B502" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A503" s="1">
+        <v>44484</v>
+      </c>
+      <c r="B503" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" s="1">
+        <v>44485</v>
+      </c>
+      <c r="B504" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A505" s="1">
+        <v>44486</v>
+      </c>
+      <c r="B505" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A506" s="1">
+        <v>44487</v>
+      </c>
+      <c r="B506" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A507" s="1">
+        <v>44488</v>
+      </c>
+      <c r="B507" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A508" s="1">
+        <v>44489</v>
+      </c>
+      <c r="B508" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A509" s="1">
+        <v>44490</v>
+      </c>
+      <c r="B509" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A510" s="1">
+        <v>44491</v>
+      </c>
+      <c r="B510" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A511" s="1">
+        <v>44492</v>
+      </c>
+      <c r="B511" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" s="1">
+        <v>44493</v>
+      </c>
+      <c r="B512" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" s="1">
+        <v>44494</v>
+      </c>
+      <c r="B513" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" s="1">
+        <v>44495</v>
+      </c>
+      <c r="B514" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" s="1">
+        <v>44496</v>
+      </c>
+      <c r="B515" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" s="1">
+        <v>44497</v>
+      </c>
+      <c r="B516" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" s="1">
+        <v>44498</v>
+      </c>
+      <c r="B517" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" s="1">
+        <v>44499</v>
+      </c>
+      <c r="B518" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A519" s="1">
+        <v>44500</v>
+      </c>
+      <c r="B519" s="2">
+        <v>1.1847713333333334</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A520" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B520">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A521" s="1">
+        <v>44502</v>
+      </c>
+      <c r="B521">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A522" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B522">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A523" s="1">
+        <v>44504</v>
+      </c>
+      <c r="B523">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A524" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B524">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A525" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B525">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A526" s="1">
+        <v>44507</v>
+      </c>
+      <c r="B526">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A527" s="1">
+        <v>44508</v>
+      </c>
+      <c r="B527">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A528" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B528">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A529" s="1">
+        <v>44510</v>
+      </c>
+      <c r="B529">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A530" s="1">
+        <v>44511</v>
+      </c>
+      <c r="B530">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A531" s="1">
+        <v>44512</v>
+      </c>
+      <c r="B531">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A532" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B532">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A533" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B533">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A534" s="1">
+        <v>44515</v>
+      </c>
+      <c r="B534">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A535" s="1">
+        <v>44516</v>
+      </c>
+      <c r="B535">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A536" s="1">
+        <v>44517</v>
+      </c>
+      <c r="B536">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A537" s="1">
+        <v>44518</v>
+      </c>
+      <c r="B537">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A538" s="1">
+        <v>44519</v>
+      </c>
+      <c r="B538">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A539" s="1">
+        <v>44520</v>
+      </c>
+      <c r="B539">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A540" s="1">
+        <v>44521</v>
+      </c>
+      <c r="B540">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A541" s="1">
+        <v>44522</v>
+      </c>
+      <c r="B541">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A542" s="1">
+        <v>44523</v>
+      </c>
+      <c r="B542">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A543" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B543">
+        <v>1.2248196666666666</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A544" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B544">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A545" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B545">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A546" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B546">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A547" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B547">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A548" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B548">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A549" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B549">
+        <v>1.22481966666667</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A550" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B550">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A551" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B551">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B552">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A553" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B553">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A554" s="1">
+        <v>44535</v>
+      </c>
+      <c r="B554">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A555" s="1">
+        <v>44536</v>
+      </c>
+      <c r="B555">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A556" s="1">
+        <v>44537</v>
+      </c>
+      <c r="B556">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A557" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B557">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A558" s="1">
+        <v>44539</v>
+      </c>
+      <c r="B558">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A559" s="1">
+        <v>44540</v>
+      </c>
+      <c r="B559">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" s="1">
+        <v>44541</v>
+      </c>
+      <c r="B560">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A561" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B561">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A562" s="1">
+        <v>44543</v>
+      </c>
+      <c r="B562">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A563" s="1">
+        <v>44544</v>
+      </c>
+      <c r="B563">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A564" s="1">
+        <v>44545</v>
+      </c>
+      <c r="B564">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A565" s="1">
+        <v>44546</v>
+      </c>
+      <c r="B565">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A566" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B566">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A567" s="1">
+        <v>44548</v>
+      </c>
+      <c r="B567">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A568" s="1">
+        <v>44549</v>
+      </c>
+      <c r="B568">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A569" s="1">
+        <v>44550</v>
+      </c>
+      <c r="B569">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A570" s="1">
+        <v>44551</v>
+      </c>
+      <c r="B570">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A571" s="1">
+        <v>44552</v>
+      </c>
+      <c r="B571">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A572" s="1">
+        <v>44553</v>
+      </c>
+      <c r="B572">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A573" s="1">
+        <v>44554</v>
+      </c>
+      <c r="B573">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A574" s="1">
+        <v>44555</v>
+      </c>
+      <c r="B574">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A575" s="1">
+        <v>44556</v>
+      </c>
+      <c r="B575">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A576" s="1">
+        <v>44557</v>
+      </c>
+      <c r="B576">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" s="1">
+        <v>44558</v>
+      </c>
+      <c r="B577">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" s="1">
+        <v>44559</v>
+      </c>
+      <c r="B578">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A579" s="1">
+        <v>44560</v>
+      </c>
+      <c r="B579">
+        <v>0.400507</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A580" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B580">
+        <v>0.400507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>